<commit_message>
v1.0 finished! Missing: better storage, y0 matching, calibration separate from data...
</commit_message>
<xml_diff>
--- a/data/cnf_files/restore_cnf_v1.xlsx
+++ b/data/cnf_files/restore_cnf_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E570750-09BF-0B47-AA8A-74CB0F32699C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E356ABD7-C4EF-7544-8D60-E58F90CA321B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="3" xr2:uid="{7D23F7FD-CED4-D849-A2DB-E011B314F00F}"/>
+    <workbookView xWindow="38420" yWindow="-4880" windowWidth="21600" windowHeight="37900" firstSheet="6" activeTab="12" xr2:uid="{7D23F7FD-CED4-D849-A2DB-E011B314F00F}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="16" r:id="rId1"/>
@@ -46,6 +46,82 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{BB00D018-43A8-3C4D-AD66-C033D854D227}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>TWh</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A41" authorId="0" shapeId="0" xr:uid="{1B4BF702-5F08-9843-A80B-5003533C2576}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>GW</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
@@ -117,11 +193,44 @@
         </r>
       </text>
     </comment>
+    <comment ref="M35" authorId="0" shapeId="0" xr:uid="{F338AE33-8AF4-E94C-9FA3-5F4CC3D9C0BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Imports, Storage and Supply</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
@@ -1025,7 +1134,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B112" sqref="B112"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1772,10 +1881,10 @@
   <dimension ref="A1:T124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M64" sqref="M64"/>
+      <selection pane="bottomRight" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2305,7 +2414,7 @@
         <v>7.4950000000000001</v>
       </c>
       <c r="M35">
-        <v>52.378999999999998</v>
+        <v>76.873000000000005</v>
       </c>
       <c r="N35">
         <v>46.578000000000003</v>
@@ -2356,7 +2465,7 @@
         <v>7.55</v>
       </c>
       <c r="M36">
-        <v>54.131999999999998</v>
+        <v>80.082999999999998</v>
       </c>
       <c r="N36">
         <v>47.585999999999999</v>
@@ -2407,7 +2516,7 @@
         <v>7.4379999999999997</v>
       </c>
       <c r="M37">
-        <v>55.91</v>
+        <v>79.105000000000004</v>
       </c>
       <c r="N37">
         <v>47.866</v>
@@ -2458,7 +2567,7 @@
         <v>7.45</v>
       </c>
       <c r="M38">
-        <v>58.127000000000002</v>
+        <v>83.167000000000002</v>
       </c>
       <c r="N38">
         <v>47.238999999999997</v>
@@ -2509,7 +2618,7 @@
         <v>7.556</v>
       </c>
       <c r="M39">
-        <v>62.39</v>
+        <v>86.384</v>
       </c>
       <c r="N39">
         <v>46.896999999999998</v>
@@ -2560,7 +2669,7 @@
         <v>7.431</v>
       </c>
       <c r="M40">
-        <v>58.838000000000001</v>
+        <v>89.305999999999997</v>
       </c>
       <c r="N40">
         <v>47.881999999999998</v>
@@ -2611,7 +2720,7 @@
         <v>7.3460000000000001</v>
       </c>
       <c r="M41">
-        <v>53.366</v>
+        <v>88.605000000000004</v>
       </c>
       <c r="N41">
         <v>48.692</v>
@@ -2662,7 +2771,7 @@
         <v>7.649</v>
       </c>
       <c r="M42">
-        <v>59.081000000000003</v>
+        <v>91.254999999999995</v>
       </c>
       <c r="N42">
         <v>48.612000000000002</v>
@@ -2713,7 +2822,7 @@
         <v>8.0809999999999995</v>
       </c>
       <c r="M43">
-        <v>59.328000000000003</v>
+        <v>98.367000000000004</v>
       </c>
       <c r="N43">
         <v>49.62</v>
@@ -2764,7 +2873,7 @@
         <v>8.7349999999999994</v>
       </c>
       <c r="M44">
-        <v>65.284999999999997</v>
+        <v>103.75700000000001</v>
       </c>
       <c r="N44">
         <v>51.213000000000001</v>
@@ -2815,7 +2924,7 @@
         <v>9.4440000000000008</v>
       </c>
       <c r="M45">
-        <v>63.374000000000002</v>
+        <v>89.677999999999997</v>
       </c>
       <c r="N45">
         <v>52.372999999999998</v>
@@ -2866,7 +2975,7 @@
         <v>9.9870000000000001</v>
       </c>
       <c r="M46">
-        <v>68.227000000000004</v>
+        <v>94.27</v>
       </c>
       <c r="N46">
         <v>53.749000000000002</v>
@@ -2917,7 +3026,7 @@
         <v>10.266</v>
       </c>
       <c r="M47">
-        <v>62.593000000000004</v>
+        <v>92.811000000000007</v>
       </c>
       <c r="N47">
         <v>54.029000000000003</v>
@@ -2968,7 +3077,7 @@
         <v>10.14</v>
       </c>
       <c r="M48">
-        <v>62.372999999999998</v>
+        <v>95.35</v>
       </c>
       <c r="N48">
         <v>55.122</v>
@@ -3019,7 +3128,7 @@
         <v>10.304</v>
       </c>
       <c r="M49">
-        <v>61.09</v>
+        <v>90.578999999999994</v>
       </c>
       <c r="N49">
         <v>56.170999999999999</v>
@@ -3070,7 +3179,7 @@
         <v>10.8</v>
       </c>
       <c r="M50">
-        <v>55.286999999999999</v>
+        <v>96.263999999999996</v>
       </c>
       <c r="N50">
         <v>57.33</v>
@@ -3121,7 +3230,7 @@
         <v>11.91</v>
       </c>
       <c r="M51">
-        <v>59.420999999999999</v>
+        <v>95.944000000000003</v>
       </c>
       <c r="N51">
         <v>57.781999999999996</v>
@@ -3172,7 +3281,7 @@
         <v>11.91</v>
       </c>
       <c r="M52">
-        <v>63.811999999999998</v>
+        <v>100.73399999999999</v>
       </c>
       <c r="N52">
         <v>57.432000000000002</v>
@@ -3223,7 +3332,7 @@
         <v>11.792</v>
       </c>
       <c r="M53">
-        <v>64.281999999999996</v>
+        <v>98.567999999999998</v>
       </c>
       <c r="N53">
         <v>58.728999999999999</v>
@@ -3274,7 +3383,7 @@
         <v>11.699</v>
       </c>
       <c r="M54">
-        <v>63.970999999999997</v>
+        <v>97.861999999999995</v>
       </c>
       <c r="N54">
         <v>57.494</v>
@@ -3325,7 +3434,7 @@
         <v>12.111000000000001</v>
       </c>
       <c r="M55">
-        <v>63.758000000000003</v>
+        <v>99.653000000000006</v>
       </c>
       <c r="N55">
         <v>59.784999999999997</v>
@@ -3376,7 +3485,7 @@
         <v>12.285</v>
       </c>
       <c r="M56">
-        <v>60.414999999999999</v>
+        <v>97.704999999999998</v>
       </c>
       <c r="N56">
         <v>58.598999999999997</v>
@@ -3427,7 +3536,7 @@
         <v>12.595000000000001</v>
       </c>
       <c r="M57">
-        <v>65.608000000000004</v>
+        <v>99.567999999999998</v>
       </c>
       <c r="N57">
         <v>58.972999999999999</v>
@@ -3478,7 +3587,7 @@
         <v>12.164</v>
       </c>
       <c r="M58">
-        <v>66.180000000000007</v>
+        <v>98.186000000000007</v>
       </c>
       <c r="N58">
         <v>59.323</v>
@@ -3529,7 +3638,7 @@
         <v>12.388999999999999</v>
       </c>
       <c r="M59">
-        <v>67.278000000000006</v>
+        <v>98.162999999999997</v>
       </c>
       <c r="N59">
         <v>57.466000000000001</v>
@@ -3580,7 +3689,7 @@
         <v>12.795999999999999</v>
       </c>
       <c r="M60">
-        <v>63.661000000000001</v>
+        <v>99.99</v>
       </c>
       <c r="N60">
         <v>58.246000000000002</v>
@@ -3631,7 +3740,7 @@
         <v>13.263</v>
       </c>
       <c r="M61">
-        <v>58.694000000000003</v>
+        <v>95.712000000000003</v>
       </c>
       <c r="N61">
         <v>58.238999999999997</v>
@@ -3682,7 +3791,7 @@
         <v>13.333</v>
       </c>
       <c r="M62">
-        <v>57.326999999999998</v>
+        <v>97.983000000000004</v>
       </c>
       <c r="N62">
         <v>58.482999999999997</v>
@@ -3733,7 +3842,7 @@
         <v>13.445</v>
       </c>
       <c r="M63">
-        <v>63.570999999999998</v>
+        <v>98.578000000000003</v>
       </c>
       <c r="N63">
         <v>57.646999999999998</v>
@@ -3781,7 +3890,7 @@
         <v>13.535</v>
       </c>
       <c r="M64">
-        <v>67.760999999999996</v>
+        <v>101.399</v>
       </c>
       <c r="N64">
         <v>57.198</v>
@@ -5381,11 +5490,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58A62B4-519C-B046-B445-0684D5B05765}">
   <dimension ref="A1:I345"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C270" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D312" sqref="D312"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5569,151 +5678,103 @@
         <v>1990</v>
       </c>
       <c r="D16">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6.54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17">
         <v>1991</v>
       </c>
-      <c r="D17">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18">
         <v>1992</v>
       </c>
-      <c r="D18">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19">
         <v>1993</v>
       </c>
-      <c r="D19">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20">
         <v>1994</v>
       </c>
-      <c r="D20">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21">
         <v>1995</v>
       </c>
-      <c r="D21">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22">
         <v>1996</v>
       </c>
-      <c r="D22">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23">
         <v>1997</v>
       </c>
-      <c r="D23">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24">
         <v>1998</v>
       </c>
-      <c r="D24">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25">
         <v>1999</v>
       </c>
-      <c r="D25">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26">
         <v>2000</v>
       </c>
-      <c r="D26">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27">
         <v>2001</v>
       </c>
-      <c r="D27">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28">
         <v>2002</v>
       </c>
-      <c r="D28">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29">
         <v>2003</v>
       </c>
-      <c r="D29">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30">
         <v>2004</v>
       </c>
-      <c r="D30">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31">
         <v>2005</v>
       </c>
-      <c r="D31">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32">
         <v>2006</v>
-      </c>
-      <c r="D32">
-        <v>9.9</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -5721,116 +5782,77 @@
       <c r="B33">
         <v>2007</v>
       </c>
-      <c r="D33">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34">
         <v>2008</v>
       </c>
-      <c r="D34">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35">
         <v>2009</v>
       </c>
-      <c r="D35">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36">
         <v>2010</v>
       </c>
-      <c r="D36">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="13"/>
       <c r="B37">
         <v>2011</v>
       </c>
-      <c r="D37">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="13"/>
       <c r="B38">
         <v>2012</v>
       </c>
-      <c r="D38">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="13"/>
       <c r="B39">
         <v>2013</v>
       </c>
-      <c r="D39">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="13"/>
       <c r="B40">
         <v>2014</v>
       </c>
-      <c r="D40">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="13"/>
       <c r="B41">
         <v>2015</v>
       </c>
-      <c r="D41">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="13"/>
       <c r="B42">
         <v>2016</v>
       </c>
-      <c r="D42">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="13"/>
       <c r="B43">
         <v>2017</v>
       </c>
-      <c r="D43">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="13"/>
       <c r="B44">
         <v>2018</v>
       </c>
-      <c r="D44">
-        <v>9.9</v>
-      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="13"/>
       <c r="B45">
         <v>2019</v>
-      </c>
-      <c r="D45">
-        <v>9.9</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -13586,7 +13608,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11:B13"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13878,17 +13900,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419CCE0D-F28F-4D4E-8D7A-EAF8794209AB}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomRight" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14014,7 +14036,7 @@
         <v>103</v>
       </c>
       <c r="M12">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -14031,7 +14053,7 @@
         <v>78</v>
       </c>
       <c r="C14">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -14040,7 +14062,7 @@
         <v>79</v>
       </c>
       <c r="D15">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -14049,7 +14071,7 @@
         <v>80</v>
       </c>
       <c r="F16">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -14058,7 +14080,7 @@
         <v>81</v>
       </c>
       <c r="H17">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -14067,7 +14089,7 @@
         <v>82</v>
       </c>
       <c r="L18">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -14076,7 +14098,7 @@
         <v>83</v>
       </c>
       <c r="E19">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -14085,7 +14107,7 @@
         <v>84</v>
       </c>
       <c r="G20">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -14094,7 +14116,7 @@
         <v>85</v>
       </c>
       <c r="G21">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -14103,7 +14125,7 @@
         <v>86</v>
       </c>
       <c r="K22">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -14112,7 +14134,7 @@
         <v>87</v>
       </c>
       <c r="I23">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -14121,7 +14143,7 @@
         <v>88</v>
       </c>
       <c r="J24">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -14132,7 +14154,7 @@
         <v>77</v>
       </c>
       <c r="M25">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -14797,7 +14819,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14956,7 +14978,7 @@
         <v>103</v>
       </c>
       <c r="M12">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -14976,7 +14998,7 @@
         <v>78</v>
       </c>
       <c r="M14">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -14985,7 +15007,7 @@
         <v>79</v>
       </c>
       <c r="M15">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -14994,7 +15016,7 @@
         <v>80</v>
       </c>
       <c r="M16">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -15003,7 +15025,7 @@
         <v>81</v>
       </c>
       <c r="M17">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -15012,7 +15034,7 @@
         <v>82</v>
       </c>
       <c r="M18">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -15021,7 +15043,7 @@
         <v>83</v>
       </c>
       <c r="M19">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -15030,7 +15052,7 @@
         <v>84</v>
       </c>
       <c r="M20">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -15039,7 +15061,7 @@
         <v>85</v>
       </c>
       <c r="M21">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -15048,7 +15070,7 @@
         <v>86</v>
       </c>
       <c r="M22">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -15057,7 +15079,7 @@
         <v>87</v>
       </c>
       <c r="M23">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -15066,7 +15088,7 @@
         <v>88</v>
       </c>
       <c r="M24">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -15077,7 +15099,7 @@
         <v>77</v>
       </c>
       <c r="M25">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -15436,14 +15458,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0549AD3-5111-4246-BF83-70CE5D37A83F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0549AD3-5111-4246-BF83-70CE5D37A83F}">
   <dimension ref="A1:M310"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D121" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F197" sqref="F197"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27558,5 +27580,6 @@
     <mergeCell ref="A251:A280"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added capacity printing functionality
</commit_message>
<xml_diff>
--- a/data/cnf_files/restore_cnf_v1.xlsx
+++ b/data/cnf_files/restore_cnf_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E356ABD7-C4EF-7544-8D60-E58F90CA321B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A498BBB-BAC8-014D-9602-1D387EBDE87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="-4880" windowWidth="21600" windowHeight="37900" firstSheet="6" activeTab="12" xr2:uid="{7D23F7FD-CED4-D849-A2DB-E011B314F00F}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" xr2:uid="{7D23F7FD-CED4-D849-A2DB-E011B314F00F}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="16" r:id="rId1"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="104">
   <si>
     <t>biogas</t>
   </si>
@@ -439,9 +439,6 @@
   </si>
   <si>
     <t>Electricity</t>
-  </si>
-  <si>
-    <t>Heat</t>
   </si>
   <si>
     <t>Primarily using D-EXPANSE data, re-arranged to an ESOM compatible format.</t>
@@ -733,11 +730,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9269511-3915-EC4F-A367-043607C24BDE}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,7 +1102,7 @@
         <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1114,11 +1111,6 @@
       </c>
       <c r="B3" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1156,26 +1148,26 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" t="s">
         <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
@@ -1956,10 +1948,10 @@
     </row>
     <row r="2" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -1968,7 +1960,7 @@
     <row r="3" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -1976,10 +1968,10 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M4">
         <v>0.2</v>
@@ -3907,7 +3899,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B65">
         <v>1990</v>
@@ -4179,7 +4171,7 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B95">
         <v>1990</v>
@@ -4530,15 +4522,15 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>26</v>
@@ -5490,7 +5482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58A62B4-519C-B046-B445-0684D5B05765}">
   <dimension ref="A1:I345"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5513,21 +5505,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
         <v>102</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>103</v>
-      </c>
-      <c r="E1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5542,7 +5534,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -5551,7 +5543,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -5560,7 +5552,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -5569,7 +5561,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -5577,7 +5569,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>45</v>
@@ -5634,7 +5626,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12">
         <v>0.4</v>
@@ -5643,7 +5635,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13">
         <v>0.4</v>
@@ -9194,15 +9186,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -9210,7 +9202,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
@@ -12033,15 +12025,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>3.5000000000000003E-2</v>
@@ -12050,7 +12042,7 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3">
         <v>-0.25</v>
@@ -12058,7 +12050,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="7">
         <v>1990</v>
@@ -12327,7 +12319,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="7">
         <v>1990</v>
@@ -12596,7 +12588,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" s="7">
         <v>1990</v>
@@ -12778,7 +12770,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B94" s="7">
         <v>1990</v>
@@ -13047,7 +13039,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B124" s="7">
         <v>1990</v>
@@ -13319,7 +13311,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B154" s="7">
         <v>1990</v>
@@ -13619,22 +13611,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="15"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -13677,174 +13669,174 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>66</v>
+      <c r="A3" s="15" t="s">
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>67</v>
+      <c r="A11" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="B11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" t="s">
-        <v>103</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>69</v>
+      <c r="A14" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14">
         <v>0.23957674956666672</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="15"/>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15">
         <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16">
         <v>0.44790000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H17">
         <v>0.2868703549999998</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L18">
         <v>0.141307988</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="15"/>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E19">
         <v>0.28399999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -13852,10 +13844,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -13863,10 +13855,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -13874,7 +13866,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -13915,22 +13907,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="15"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -13973,174 +13965,174 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>66</v>
+      <c r="A3" s="15" t="s">
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>67</v>
+      <c r="A11" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="B11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" t="s">
-        <v>103</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>69</v>
+      <c r="A14" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="15"/>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="15"/>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -14148,10 +14140,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -14159,10 +14151,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -14170,7 +14162,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -14211,22 +14203,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="15"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -14269,174 +14261,174 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>66</v>
+      <c r="A3" s="15" t="s">
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>67</v>
+      <c r="A11" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="B11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" t="s">
-        <v>103</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>69</v>
+      <c r="A14" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="15"/>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="15"/>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -14444,10 +14436,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -14455,10 +14447,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -14466,7 +14458,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -14507,22 +14499,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="15"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -14565,8 +14557,8 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>66</v>
+      <c r="A3" s="15" t="s">
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -14576,7 +14568,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -14585,7 +14577,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -14594,7 +14586,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -14603,7 +14595,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -14612,7 +14604,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -14621,7 +14613,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -14630,7 +14622,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -14639,130 +14631,130 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>72</v>
+      <c r="A11" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="15"/>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>69</v>
+      <c r="A14" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M14">
         <v>0.95</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="15"/>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M15">
         <v>0.9</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M16">
         <v>0.95</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M17">
         <v>0.95</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M18">
         <v>0.73924900000000004</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="15"/>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M19">
         <v>0.95</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M20">
         <v>0.98</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M21">
         <v>0.98</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M22">
         <v>0.98</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -14770,10 +14762,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M25">
         <v>0.73</v>
@@ -14781,10 +14773,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N26">
         <v>0.91</v>
@@ -14792,7 +14784,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -14830,22 +14822,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="15"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -14888,8 +14880,8 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>66</v>
+      <c r="A3" s="15" t="s">
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -14899,7 +14891,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -14908,7 +14900,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -14917,7 +14909,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -14926,7 +14918,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -14935,7 +14927,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -14944,7 +14936,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -14953,7 +14945,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -14962,130 +14954,130 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>72</v>
+      <c r="A11" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="15"/>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>69</v>
+      <c r="A14" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="15"/>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="15"/>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -15093,10 +15085,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -15104,10 +15096,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -15115,7 +15107,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -15153,22 +15145,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="15"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -15211,8 +15203,8 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>66</v>
+      <c r="A3" s="15" t="s">
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -15222,7 +15214,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -15231,7 +15223,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -15240,7 +15232,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -15249,7 +15241,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -15258,7 +15250,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -15267,7 +15259,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -15276,7 +15268,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -15285,130 +15277,130 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>72</v>
+      <c r="A11" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="15"/>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>69</v>
+      <c r="A14" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="15"/>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="15"/>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -15416,10 +15408,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -15427,10 +15419,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -15438,7 +15430,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -15487,45 +15479,45 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>79</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>81</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>82</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>83</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>84</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>85</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>86</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>87</v>
-      </c>
-      <c r="M1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -15563,7 +15555,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
@@ -27567,17 +27559,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A11:A40"/>
-    <mergeCell ref="A41:A70"/>
-    <mergeCell ref="A71:A100"/>
-    <mergeCell ref="A101:A130"/>
     <mergeCell ref="A281:A310"/>
     <mergeCell ref="A131:A160"/>
     <mergeCell ref="A161:A190"/>
     <mergeCell ref="A191:A220"/>
     <mergeCell ref="A221:A250"/>
     <mergeCell ref="A251:A280"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A11:A40"/>
+    <mergeCell ref="A41:A70"/>
+    <mergeCell ref="A71:A100"/>
+    <mergeCell ref="A101:A130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
small checkpoint before working on file conversion
</commit_message>
<xml_diff>
--- a/data/cnf_files/restore_cnf_v1.xlsx
+++ b/data/cnf_files/restore_cnf_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A498BBB-BAC8-014D-9602-1D387EBDE87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62B432F-53A6-4A4A-979C-D24E99598BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" xr2:uid="{7D23F7FD-CED4-D849-A2DB-E011B314F00F}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" firstSheet="4" activeTab="10" xr2:uid="{7D23F7FD-CED4-D849-A2DB-E011B314F00F}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="16" r:id="rId1"/>
@@ -46,6 +46,49 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="A184" authorId="0" shapeId="0" xr:uid="{3AFFE9DF-411A-0541-8926-EC93AA292287}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>tco2</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
@@ -121,7 +164,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
@@ -230,7 +273,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
@@ -274,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="106">
   <si>
     <t>biogas</t>
   </si>
@@ -586,6 +629,12 @@
   </si>
   <si>
     <t>trd_gas</t>
+  </si>
+  <si>
+    <t>actual_emissions_elec_heat</t>
+  </si>
+  <si>
+    <t>actual_co2_emissions</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9269511-3915-EC4F-A367-043607C24BDE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1870,13 +1919,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0FB1D5-567E-D142-9CEC-119D006AC3BA}">
-  <dimension ref="A1:T124"/>
+  <dimension ref="A1:T154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="L92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N35" sqref="N35"/>
+      <selection pane="bottomRight" activeCell="N136" sqref="N136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4441,8 +4490,281 @@
         <v>9.8030000000000008</v>
       </c>
     </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A125" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B125">
+        <v>1990</v>
+      </c>
+      <c r="M125">
+        <v>244310</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A126" s="13"/>
+      <c r="B126">
+        <v>1991</v>
+      </c>
+      <c r="M126">
+        <v>410930</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A127" s="13"/>
+      <c r="B127">
+        <v>1992</v>
+      </c>
+      <c r="M127">
+        <v>515700</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A128" s="13"/>
+      <c r="B128">
+        <v>1993</v>
+      </c>
+      <c r="M128">
+        <v>179200</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A129" s="13"/>
+      <c r="B129">
+        <v>1994</v>
+      </c>
+      <c r="M129">
+        <v>155720</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A130" s="13"/>
+      <c r="B130">
+        <v>1995</v>
+      </c>
+      <c r="M130">
+        <v>146530</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A131" s="13"/>
+      <c r="B131">
+        <v>1996</v>
+      </c>
+      <c r="M131">
+        <v>193790</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A132" s="13"/>
+      <c r="B132">
+        <v>1997</v>
+      </c>
+      <c r="M132">
+        <v>88850</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A133" s="13"/>
+      <c r="B133">
+        <v>1998</v>
+      </c>
+      <c r="M133">
+        <v>320440</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A134" s="13"/>
+      <c r="B134">
+        <v>1999</v>
+      </c>
+      <c r="M134">
+        <v>132260</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A135" s="13"/>
+      <c r="B135">
+        <v>2000</v>
+      </c>
+      <c r="M135">
+        <v>60820</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A136" s="13"/>
+      <c r="B136">
+        <v>2001</v>
+      </c>
+      <c r="M136">
+        <v>64670</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A137" s="13"/>
+      <c r="B137">
+        <v>2002</v>
+      </c>
+      <c r="M137">
+        <v>66110</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A138" s="13"/>
+      <c r="B138">
+        <v>2003</v>
+      </c>
+      <c r="M138">
+        <v>75150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A139" s="13"/>
+      <c r="B139">
+        <v>2004</v>
+      </c>
+      <c r="M139">
+        <v>60790</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A140" s="13"/>
+      <c r="B140">
+        <v>2005</v>
+      </c>
+      <c r="M140">
+        <v>79820</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A141" s="13"/>
+      <c r="B141">
+        <v>2006</v>
+      </c>
+      <c r="M141">
+        <v>77640</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A142" s="13"/>
+      <c r="B142">
+        <v>2007</v>
+      </c>
+      <c r="M142">
+        <v>68530</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A143" s="13"/>
+      <c r="B143">
+        <v>2008</v>
+      </c>
+      <c r="M143">
+        <v>43340</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A144" s="13"/>
+      <c r="B144">
+        <v>2009</v>
+      </c>
+      <c r="M144">
+        <v>36540</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A145" s="13"/>
+      <c r="B145">
+        <v>2010</v>
+      </c>
+      <c r="M145">
+        <v>22980</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A146" s="13"/>
+      <c r="B146">
+        <v>2011</v>
+      </c>
+      <c r="M146">
+        <v>14040</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A147" s="13"/>
+      <c r="B147">
+        <v>2012</v>
+      </c>
+      <c r="M147">
+        <v>12530</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A148" s="13"/>
+      <c r="B148">
+        <v>2013</v>
+      </c>
+      <c r="M148">
+        <v>11790</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A149" s="13"/>
+      <c r="B149">
+        <v>2014</v>
+      </c>
+      <c r="M149">
+        <v>8840</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A150" s="13"/>
+      <c r="B150">
+        <v>2015</v>
+      </c>
+      <c r="M150">
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A151" s="13"/>
+      <c r="B151">
+        <v>2016</v>
+      </c>
+      <c r="M151">
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A152" s="13"/>
+      <c r="B152">
+        <v>2017</v>
+      </c>
+      <c r="M152">
+        <v>11790</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A153" s="13"/>
+      <c r="B153">
+        <v>2018</v>
+      </c>
+      <c r="M153">
+        <v>9580</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A154" s="13"/>
+      <c r="B154">
+        <v>2019</v>
+      </c>
+      <c r="M154">
+        <v>11790</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A125:A154"/>
     <mergeCell ref="A65:A94"/>
     <mergeCell ref="A95:A124"/>
     <mergeCell ref="A5:A34"/>
@@ -12007,14 +12329,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667431D6-B9A7-2740-A47A-09D6E50D45F6}">
-  <dimension ref="A1:C183"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667431D6-B9A7-2740-A47A-09D6E50D45F6}">
+  <dimension ref="A1:C213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C182" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13578,8 +13900,281 @@
         <v>2019</v>
       </c>
     </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B184" s="7">
+        <v>1990</v>
+      </c>
+      <c r="C184" s="7">
+        <v>2519999.9810000001</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="12"/>
+      <c r="B185" s="7">
+        <v>1991</v>
+      </c>
+      <c r="C185" s="7">
+        <v>3039999.9619999998</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="12"/>
+      <c r="B186" s="7">
+        <v>1992</v>
+      </c>
+      <c r="C186" s="7">
+        <v>3170000.0759999999</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" s="12"/>
+      <c r="B187" s="7">
+        <v>1993</v>
+      </c>
+      <c r="C187" s="7">
+        <v>2829999.9240000001</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="12"/>
+      <c r="B188" s="7">
+        <v>1994</v>
+      </c>
+      <c r="C188" s="7">
+        <v>3019999.9810000001</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" s="12"/>
+      <c r="B189" s="7">
+        <v>1995</v>
+      </c>
+      <c r="C189" s="7">
+        <v>2880000.1140000001</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="12"/>
+      <c r="B190" s="7">
+        <v>1996</v>
+      </c>
+      <c r="C190" s="7">
+        <v>2970000.0290000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="12"/>
+      <c r="B191" s="7">
+        <v>1997</v>
+      </c>
+      <c r="C191" s="7">
+        <v>3170000.0759999999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="12"/>
+      <c r="B192" s="7">
+        <v>1998</v>
+      </c>
+      <c r="C192" s="7">
+        <v>3690000.057</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" s="12"/>
+      <c r="B193" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C193" s="7">
+        <v>3470000.0290000001</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" s="12"/>
+      <c r="B194" s="7">
+        <v>2000</v>
+      </c>
+      <c r="C194" s="7">
+        <v>3329999.9240000001</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" s="12"/>
+      <c r="B195" s="7">
+        <v>2001</v>
+      </c>
+      <c r="C195" s="7">
+        <v>3480000.0189999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" s="12"/>
+      <c r="B196" s="7">
+        <v>2002</v>
+      </c>
+      <c r="C196" s="7">
+        <v>3559999.943</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" s="12"/>
+      <c r="B197" s="7">
+        <v>2003</v>
+      </c>
+      <c r="C197" s="7">
+        <v>3579999.9240000001</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" s="12"/>
+      <c r="B198" s="7">
+        <v>2004</v>
+      </c>
+      <c r="C198" s="7">
+        <v>3970000.0290000001</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="12"/>
+      <c r="B199" s="7">
+        <v>2005</v>
+      </c>
+      <c r="C199" s="7">
+        <v>4070000.1719999998</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" s="12"/>
+      <c r="B200" s="7">
+        <v>2006</v>
+      </c>
+      <c r="C200" s="7">
+        <v>4179999.8280000002</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" s="12"/>
+      <c r="B201" s="7">
+        <v>2007</v>
+      </c>
+      <c r="C201" s="7">
+        <v>3839999.9139999999</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" s="12"/>
+      <c r="B202" s="7">
+        <v>2008</v>
+      </c>
+      <c r="C202" s="7">
+        <v>3940000.057</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" s="12"/>
+      <c r="B203" s="7">
+        <v>2009</v>
+      </c>
+      <c r="C203" s="7">
+        <v>3660000.0860000001</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" s="12"/>
+      <c r="B204" s="7">
+        <v>2010</v>
+      </c>
+      <c r="C204" s="7">
+        <v>3829999.9240000001</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" s="12"/>
+      <c r="B205" s="7">
+        <v>2011</v>
+      </c>
+      <c r="C205" s="7">
+        <v>3650000.0950000002</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" s="12"/>
+      <c r="B206" s="7">
+        <v>2012</v>
+      </c>
+      <c r="C206" s="7">
+        <v>3619999.8859999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" s="12"/>
+      <c r="B207" s="7">
+        <v>2013</v>
+      </c>
+      <c r="C207" s="7">
+        <v>3740000.01</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" s="12"/>
+      <c r="B208" s="7">
+        <v>2014</v>
+      </c>
+      <c r="C208" s="7">
+        <v>3609999.895</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" s="12"/>
+      <c r="B209" s="7">
+        <v>2015</v>
+      </c>
+      <c r="C209" s="7">
+        <v>3119999.8859999999</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" s="12"/>
+      <c r="B210" s="7">
+        <v>2016</v>
+      </c>
+      <c r="C210" s="7">
+        <v>3200000.048</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" s="12"/>
+      <c r="B211" s="7">
+        <v>2017</v>
+      </c>
+      <c r="C211" s="7">
+        <v>3190000.057</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" s="12"/>
+      <c r="B212" s="7">
+        <v>2018</v>
+      </c>
+      <c r="C212" s="7">
+        <v>3180000.0669999998</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" s="12"/>
+      <c r="B213" s="7">
+        <v>2019</v>
+      </c>
+      <c r="C213" s="7">
+        <v>3190000.057</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A184:A213"/>
     <mergeCell ref="A154:A183"/>
     <mergeCell ref="A94:A123"/>
     <mergeCell ref="A4:A33"/>
@@ -13589,6 +14184,7 @@
     <mergeCell ref="A124:A153"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15457,7 +16053,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Before testing configuration file generation
</commit_message>
<xml_diff>
--- a/data/cnf_files/restore_cnf_v1.xlsx
+++ b/data/cnf_files/restore_cnf_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62B432F-53A6-4A4A-979C-D24E99598BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C62D23-582E-D242-9FB1-5490C6D0DE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" firstSheet="4" activeTab="10" xr2:uid="{7D23F7FD-CED4-D849-A2DB-E011B314F00F}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="17500" windowHeight="19900" firstSheet="1" activeTab="5" xr2:uid="{7D23F7FD-CED4-D849-A2DB-E011B314F00F}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="16" r:id="rId1"/>
@@ -1921,11 +1921,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0FB1D5-567E-D142-9CEC-119D006AC3BA}">
   <dimension ref="A1:T154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L92" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N136" sqref="N136"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4764,12 +4764,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="A125:A154"/>
     <mergeCell ref="A65:A94"/>
     <mergeCell ref="A95:A124"/>
     <mergeCell ref="A5:A34"/>
     <mergeCell ref="A35:A64"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <conditionalFormatting sqref="T5:T32">
     <cfRule type="expression" dxfId="4" priority="30">
@@ -14196,13 +14196,13 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14489,10 +14489,10 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N25" sqref="N25"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15080,11 +15080,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2D8252-A794-8B44-811E-A87F37F57892}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11:B13"/>
+      <selection pane="bottomRight" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16053,7 +16053,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28155,17 +28155,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A11:A40"/>
+    <mergeCell ref="A41:A70"/>
+    <mergeCell ref="A71:A100"/>
+    <mergeCell ref="A101:A130"/>
     <mergeCell ref="A281:A310"/>
     <mergeCell ref="A131:A160"/>
     <mergeCell ref="A161:A190"/>
     <mergeCell ref="A191:A220"/>
     <mergeCell ref="A221:A250"/>
     <mergeCell ref="A251:A280"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A11:A40"/>
-    <mergeCell ref="A41:A70"/>
-    <mergeCell ref="A71:A100"/>
-    <mergeCell ref="A101:A130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>